<commit_message>
atualização do DF add ao estado de GO
</commit_message>
<xml_diff>
--- a/output/estat-desc-xco2.xlsx
+++ b/output/estat-desc-xco2.xlsx
@@ -429,34 +429,34 @@
         </is>
       </c>
       <c r="C2">
-        <v>12402</v>
+        <v>12548</v>
       </c>
       <c r="D2">
         <v>393.2996520996094</v>
       </c>
       <c r="E2">
-        <v>398.9232358078941</v>
+        <v>398.9145028330469</v>
       </c>
       <c r="F2">
-        <v>398.9433746337891</v>
+        <v>398.9312744140625</v>
       </c>
       <c r="G2">
         <v>405.4674987792969</v>
       </c>
       <c r="H2">
-        <v>2.139899125300313</v>
+        <v>2.132369496561104</v>
       </c>
       <c r="I2">
-        <v>1.462839405163914</v>
+        <v>1.460263502440948</v>
       </c>
       <c r="J2">
-        <v>0.3666969666987159</v>
+        <v>0.366059266351641</v>
       </c>
       <c r="K2">
-        <v>-0.1686960358540144</v>
+        <v>-0.1592442942796279</v>
       </c>
       <c r="L2">
-        <v>0.8019487797666405</v>
+        <v>0.7963502066840924</v>
       </c>
     </row>
     <row r="3">
@@ -629,34 +629,34 @@
         </is>
       </c>
       <c r="C7">
-        <v>14497</v>
+        <v>14714</v>
       </c>
       <c r="D7">
         <v>394.3099975585938</v>
       </c>
       <c r="E7">
-        <v>402.2568704989677</v>
+        <v>402.2692439815702</v>
       </c>
       <c r="F7">
-        <v>402.3330993652344</v>
+        <v>402.34423828125</v>
       </c>
       <c r="G7">
         <v>409.4591674804688</v>
       </c>
       <c r="H7">
-        <v>1.924261814594852</v>
+        <v>1.935110439601139</v>
       </c>
       <c r="I7">
-        <v>1.387177643488696</v>
+        <v>1.391082470452827</v>
       </c>
       <c r="J7">
-        <v>0.3448487136510589</v>
+        <v>0.3458088062324144</v>
       </c>
       <c r="K7">
-        <v>-0.1123630459413932</v>
+        <v>-0.1066689038923072</v>
       </c>
       <c r="L7">
-        <v>0.7697158807379352</v>
+        <v>0.7729680457828501</v>
       </c>
     </row>
     <row r="8">
@@ -829,34 +829,34 @@
         </is>
       </c>
       <c r="C12">
-        <v>8862</v>
+        <v>8879</v>
       </c>
       <c r="D12">
         <v>397.3831787109375</v>
       </c>
       <c r="E12">
-        <v>404.0179888519308</v>
+        <v>404.0198314970497</v>
       </c>
       <c r="F12">
-        <v>404.0206604003906</v>
+        <v>404.0214538574219</v>
       </c>
       <c r="G12">
         <v>411.6748046875</v>
       </c>
       <c r="H12">
-        <v>1.642559298124903</v>
+        <v>1.645235531872815</v>
       </c>
       <c r="I12">
-        <v>1.281623695990716</v>
+        <v>1.28266735043534</v>
       </c>
       <c r="J12">
-        <v>0.3172194633294955</v>
+        <v>0.3174763341894781</v>
       </c>
       <c r="K12">
-        <v>0.2656912904095874</v>
+        <v>0.2639047614576369</v>
       </c>
       <c r="L12">
-        <v>1.999953672167659</v>
+        <v>1.982068610517871</v>
       </c>
     </row>
     <row r="13">
@@ -1029,34 +1029,34 @@
         </is>
       </c>
       <c r="C17">
-        <v>12582</v>
+        <v>12952</v>
       </c>
       <c r="D17">
         <v>398.5687561035156</v>
       </c>
       <c r="E17">
-        <v>406.1778782383851</v>
+        <v>406.1755092778715</v>
       </c>
       <c r="F17">
-        <v>406.3043365478516</v>
+        <v>406.2969665527344</v>
       </c>
       <c r="G17">
         <v>412.3593139648438</v>
       </c>
       <c r="H17">
-        <v>1.906164678912099</v>
+        <v>1.87967308393604</v>
       </c>
       <c r="I17">
-        <v>1.380639228369272</v>
+        <v>1.371011700874956</v>
       </c>
       <c r="J17">
-        <v>0.3399100006029814</v>
+        <v>0.3375416955375869</v>
       </c>
       <c r="K17">
-        <v>-0.5337360370023955</v>
+        <v>-0.5283813453827979</v>
       </c>
       <c r="L17">
-        <v>1.584909959036459</v>
+        <v>1.614059594151295</v>
       </c>
     </row>
     <row r="18">
@@ -1229,34 +1229,34 @@
         </is>
       </c>
       <c r="C22">
-        <v>10797</v>
+        <v>11189</v>
       </c>
       <c r="D22">
         <v>401.9984130859375</v>
       </c>
       <c r="E22">
-        <v>408.8346308321051</v>
+        <v>408.8485073219495</v>
       </c>
       <c r="F22">
-        <v>408.9322509765625</v>
+        <v>408.9463195800781</v>
       </c>
       <c r="G22">
         <v>416.2995300292969</v>
       </c>
       <c r="H22">
-        <v>2.452241739993066</v>
+        <v>2.421529258660425</v>
       </c>
       <c r="I22">
-        <v>1.565963518091359</v>
+        <v>1.556126363333141</v>
       </c>
       <c r="J22">
-        <v>0.3830310350432247</v>
+        <v>0.3806119712961951</v>
       </c>
       <c r="K22">
-        <v>-0.3872823134757487</v>
+        <v>-0.3847638769677218</v>
       </c>
       <c r="L22">
-        <v>1.536864144119347</v>
+        <v>1.605163876050673</v>
       </c>
     </row>
     <row r="23">
@@ -1429,34 +1429,34 @@
         </is>
       </c>
       <c r="C27">
-        <v>13266</v>
+        <v>13658</v>
       </c>
       <c r="D27">
         <v>405.22607421875</v>
       </c>
       <c r="E27">
-        <v>410.9890267521516</v>
+        <v>410.9726019404192</v>
       </c>
       <c r="F27">
-        <v>410.9436950683594</v>
+        <v>410.9277038574219</v>
       </c>
       <c r="G27">
         <v>416.8045349121094</v>
       </c>
       <c r="H27">
-        <v>1.854593203293101</v>
+        <v>1.861093948299786</v>
       </c>
       <c r="I27">
-        <v>1.361834499230028</v>
+        <v>1.36421917165087</v>
       </c>
       <c r="J27">
-        <v>0.3313554403123486</v>
+        <v>0.3319489341162085</v>
       </c>
       <c r="K27">
-        <v>0.08533500314030823</v>
+        <v>0.08328362086594324</v>
       </c>
       <c r="L27">
-        <v>0.4329278630243492</v>
+        <v>0.4182223542257963</v>
       </c>
     </row>
     <row r="28">

</xml_diff>